<commit_message>
Attendance taking feature added to the system
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
   <si>
     <t>Roll Number</t>
   </si>
@@ -26,142 +26,106 @@
     <t>Last Name</t>
   </si>
   <si>
-    <t>26_12_18</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>jiou</t>
-  </si>
-  <si>
-    <t>amba</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>jgjm</t>
-  </si>
-  <si>
-    <t>jmgmj</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>huiawi</t>
-  </si>
-  <si>
-    <t>gyuoi</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>jgjg</t>
-  </si>
-  <si>
-    <t>kj</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>kaju</t>
-  </si>
-  <si>
-    <t>bhaiyya</t>
+    <t>28_12_18</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>Yash</t>
+  </si>
+  <si>
+    <t>Atre</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Devender</t>
+  </si>
+  <si>
+    <t>Singh</t>
   </si>
   <si>
     <t>34</t>
   </si>
   <si>
-    <t>kittu</t>
-  </si>
-  <si>
-    <t>pilot</t>
+    <t>krutik</t>
+  </si>
+  <si>
+    <t>pathak</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>Manas</t>
+  </si>
+  <si>
+    <t>Jain</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Akshat</t>
+  </si>
+  <si>
+    <t>Gupta</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>Sakina</t>
+  </si>
+  <si>
+    <t>Saifee</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>Shubham</t>
+  </si>
+  <si>
+    <t>Pandey</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>Shweta</t>
+  </si>
+  <si>
+    <t>Solanki</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Aman</t>
+  </si>
+  <si>
+    <t>Bhawsar</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>syed</t>
+  </si>
+  <si>
+    <t>mustafa</t>
   </si>
   <si>
     <t>55</t>
   </si>
   <si>
-    <t>ghjgjh</t>
-  </si>
-  <si>
-    <t>jgjmg</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
-    <t>hfh</t>
-  </si>
-  <si>
-    <t>hyfh</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>modi</t>
-  </si>
-  <si>
-    <t>jhgj</t>
-  </si>
-  <si>
-    <t>87</t>
-  </si>
-  <si>
-    <t>hfhgd</t>
-  </si>
-  <si>
-    <t>hgjhd</t>
-  </si>
-  <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>lkhku</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>99</t>
-  </si>
-  <si>
-    <t>jigyasa</t>
-  </si>
-  <si>
-    <t>pyari</t>
-  </si>
-  <si>
-    <t>67</t>
-  </si>
-  <si>
-    <t>kio</t>
-  </si>
-  <si>
-    <t>amaar</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>kaparo</t>
-  </si>
-  <si>
-    <t>hui</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>pulsar</t>
-  </si>
-  <si>
-    <t>ghanta</t>
+    <t>palak</t>
+  </si>
+  <si>
+    <t>agrawal</t>
   </si>
 </sst>
 </file>
@@ -497,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +493,9 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
@@ -540,6 +507,9 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
@@ -551,6 +521,9 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
@@ -562,6 +535,9 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
@@ -573,6 +549,9 @@
       <c r="C7" t="s">
         <v>18</v>
       </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
@@ -584,6 +563,9 @@
       <c r="C8" t="s">
         <v>21</v>
       </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
@@ -606,6 +588,9 @@
       <c r="C10" t="s">
         <v>27</v>
       </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
@@ -617,6 +602,9 @@
       <c r="C11" t="s">
         <v>30</v>
       </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
@@ -628,6 +616,9 @@
       <c r="C12" t="s">
         <v>33</v>
       </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
@@ -639,49 +630,8 @@
       <c r="C13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
+      <c r="D13" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
attendance taking system added
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -65,6 +65,15 @@
     <t>Jain</t>
   </si>
   <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>palak</t>
+  </si>
+  <si>
+    <t>agrawal</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
@@ -117,15 +126,6 @@
   </si>
   <si>
     <t>mustafa</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>palak</t>
-  </si>
-  <si>
-    <t>agrawal</t>
   </si>
 </sst>
 </file>
@@ -577,6 +577,9 @@
       <c r="C9" t="s">
         <v>24</v>
       </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
@@ -587,9 +590,6 @@
       </c>
       <c r="C10" t="s">
         <v>27</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4">

</xml_diff>